<commit_message>
1. New screenshots for version 1.1.0.
2. A small fix to avoid abnormal climb values when calibrating the altitude.
</commit_message>
<xml_diff>
--- a/doc/Color.xlsx
+++ b/doc/Color.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="18">
   <si>
     <t>[Color]</t>
   </si>
@@ -35,14 +35,64 @@
   </si>
   <si>
     <t>Blue</t>
+  </si>
+  <si>
+    <t>Version 1.0.0 colors (Trønder-colors)</t>
+  </si>
+  <si>
+    <t>; magenta</t>
+  </si>
+  <si>
+    <t>; red</t>
+  </si>
+  <si>
+    <t>; black</t>
+  </si>
+  <si>
+    <t>; green</t>
+  </si>
+  <si>
+    <t>; cyan</t>
+  </si>
+  <si>
+    <t>; blue-magenta</t>
+  </si>
+  <si>
+    <t>; blue</t>
+  </si>
+  <si>
+    <t>; yellow</t>
+  </si>
+  <si>
+    <t>; orange</t>
+  </si>
+  <si>
+    <t>Version 1.1.0 colors</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -67,15 +117,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -375,7 +429,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -383,54 +437,44 @@
   <cols>
     <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2">
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
         <v>-10</v>
       </c>
-      <c r="C3">
-        <v>255</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2">
-        <v>-4</v>
-      </c>
       <c r="C4">
         <v>255</v>
       </c>
@@ -440,8 +484,11 @@
       <c r="E4">
         <v>255</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -455,129 +502,522 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="2">
+        <v>-4</v>
+      </c>
+      <c r="C6">
+        <v>165</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>255</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2">
+        <v>-3</v>
+      </c>
+      <c r="C7">
+        <v>165</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>255</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2">
+        <v>-3</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>255</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="2">
         <v>-2</v>
       </c>
-      <c r="C6">
-        <v>255</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="2">
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>255</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2">
         <v>-1</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="2">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="2">
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2">
         <v>1</v>
       </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>255</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="2">
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>255</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="2">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>255</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="2">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>255</v>
+      </c>
+      <c r="D14">
+        <v>255</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="2">
         <v>4</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>255</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="2">
+      <c r="C15">
+        <v>255</v>
+      </c>
+      <c r="D15">
+        <v>255</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="2">
         <v>4</v>
       </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>255</v>
-      </c>
-      <c r="E11">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="2">
+      <c r="C16">
+        <v>255</v>
+      </c>
+      <c r="D16">
+        <v>165</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="2">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>255</v>
+      </c>
+      <c r="D17">
+        <v>165</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="2">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <v>255</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="2">
         <v>10</v>
       </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>255</v>
-      </c>
-      <c r="E12">
-        <v>255</v>
+      <c r="C19">
+        <v>255</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="2">
+        <v>-10</v>
+      </c>
+      <c r="C24">
+        <v>255</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>255</v>
+      </c>
+      <c r="F24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="2">
+        <v>-4</v>
+      </c>
+      <c r="C25">
+        <v>255</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>255</v>
+      </c>
+      <c r="F25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="2">
+        <v>-4</v>
+      </c>
+      <c r="C26">
+        <v>255</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="2">
+        <v>-2</v>
+      </c>
+      <c r="C27">
+        <v>255</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="2">
+        <v>-1</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="2">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="2">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>255</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" s="2">
+        <v>4</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>255</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="2">
+        <v>4</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>255</v>
+      </c>
+      <c r="E32">
+        <v>255</v>
+      </c>
+      <c r="F32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="2">
+        <v>10</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>255</v>
+      </c>
+      <c r="E33">
+        <v>255</v>
+      </c>
+      <c r="F33" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>